<commit_message>
BBDC4 trocado por BBDC3
</commit_message>
<xml_diff>
--- a/listaAtivos.xlsx
+++ b/listaAtivos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viniv\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vinicius\github\PortfolioAlgGen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C877CD71-9A19-44B5-AE07-F759BB0B409B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95938C22-866C-4B90-A2F8-1DB9F3601CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24310" yWindow="3970" windowWidth="29130" windowHeight="13890" xr2:uid="{A38C9114-5A97-4329-B27A-556872047A76}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{A38C9114-5A97-4329-B27A-556872047A76}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>ABEV3.SA</t>
   </si>
   <si>
-    <t>BBDC4.SA</t>
-  </si>
-  <si>
     <t>UGPA3.SA</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>RAIL3.SA</t>
+  </si>
+  <si>
+    <t>BBDC3.SA</t>
   </si>
 </sst>
 </file>
@@ -191,7 +191,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -489,148 +489,148 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069BCB45-EFD5-4423-8E07-AE8B12EDAEF7}">
   <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.796875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>